<commit_message>
Fix value for R7 and R20 in the BOM
</commit_message>
<xml_diff>
--- a/docs/bom.xlsx
+++ b/docs/bom.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -250,7 +250,7 @@
     <t xml:space="preserve">R7, R20</t>
   </si>
   <si>
-    <t xml:space="preserve">4K7 1/4W 5%</t>
+    <t xml:space="preserve">4K3 1/4W 5%</t>
   </si>
   <si>
     <t xml:space="preserve">Were 1K in the original</t>
@@ -354,6 +354,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -376,12 +377,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -432,36 +435,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -538,580 +545,580 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:E47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="49.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="49.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5" t="n">
+      <c r="B17" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="5" t="n">
+      <c r="B31" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="5" t="n">
+      <c r="B33" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="5" t="n">
+      <c r="B34" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B37" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B41" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="5" t="n">
+      <c r="B42" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="5" t="n">
+      <c r="B44" s="6" t="n">
         <v>41</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="7" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B45" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="B47" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="2" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1120,8 +1127,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>